<commit_message>
criando um robo capaz de ler pdfs e converter em xlsx
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Remédio</t>
+          <t>Cursos</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -586,40 +586,6 @@
         </is>
       </c>
       <c r="C10" t="inlineStr">
-        <is>
-          <t>Cartão</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Nova Linha 1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>220</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Cartão</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Petshop</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
         <is>
           <t>Cartão</t>
         </is>

</xml_diff>